<commit_message>
Added GUI component to document
</commit_message>
<xml_diff>
--- a/GUI_Mockups/Excel Example.xlsx
+++ b/GUI_Mockups/Excel Example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vitaliy\Documents\GitHub\Porter-Simulation\GUI Mockups\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vitaliy\Documents\GitHub\Porter-Simulation\GUI_Mockups\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Porter Simulation</t>
   </si>
@@ -72,19 +72,52 @@
   </si>
   <si>
     <t>5 minutes</t>
+  </si>
+  <si>
+    <t>Hint</t>
+  </si>
+  <si>
+    <t>min: 0 max: 200</t>
+  </si>
+  <si>
+    <t>must be more than or equal to Start Date</t>
+  </si>
+  <si>
+    <t>must be less than or equal to End Time</t>
+  </si>
+  <si>
+    <t>must be less than or equal to End Date</t>
+  </si>
+  <si>
+    <t>must be more than or equal to Start Time</t>
+  </si>
+  <si>
+    <t>Choose from Available List</t>
+  </si>
+  <si>
+    <t>min: 0% max: 100%</t>
+  </si>
+  <si>
+    <t>min: 0 max: 60 min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,14 +168,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -156,7 +183,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -176,7 +212,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" max="30000" page="10"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" max="30000" page="10" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -188,11 +224,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" max="30000" page="10"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" max="30000" page="10" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" max="30000" page="10"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" max="30000" page="10" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
@@ -203,12 +239,16 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" max="30000" page="10"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" max="30000" page="10" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" max="30000" page="10"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" max="30000" page="10" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -220,7 +260,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" max="30000" page="10"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" max="30000" page="10" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
@@ -921,15 +961,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>16933</xdr:colOff>
+          <xdr:colOff>15240</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>14394</xdr:rowOff>
+          <xdr:rowOff>15240</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
           <xdr:colOff>556260</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>166794</xdr:rowOff>
+          <xdr:rowOff>167640</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1037,6 +1077,71 @@
                   <a:latin typeface="Calibri"/>
                 </a:rPr>
                 <a:t>Advanced Setting</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>22860</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>20955</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>579120</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>150495</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1052" name="Button 28" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1052"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri"/>
+                </a:rPr>
+                <a:t>Default Settings</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -1312,136 +1417,209 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F1:I13"/>
+  <dimension ref="F1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.77734375" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F1" s="1" t="s">
+    <row r="1" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="F1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F2" s="1" t="s">
+    <row r="2" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="6:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F3" s="2" t="s">
+    <row r="3" spans="6:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="3">
+      <c r="G3" s="6"/>
+      <c r="H3" s="1">
         <v>50</v>
       </c>
+      <c r="J3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="6:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F4" s="2" t="s">
+    <row r="4" spans="6:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="4">
+      <c r="G4" s="6"/>
+      <c r="H4" s="2">
         <v>41743</v>
       </c>
+      <c r="J4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
     </row>
-    <row r="5" spans="6:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F5" s="2" t="s">
+    <row r="5" spans="6:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="5">
+      <c r="G5" s="6"/>
+      <c r="H5" s="3">
         <f>TIME(7,30,20)</f>
         <v>0.3127314814814815</v>
       </c>
+      <c r="J5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
     </row>
-    <row r="6" spans="6:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F6" s="2" t="s">
+    <row r="6" spans="6:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="4">
+      <c r="G6" s="6"/>
+      <c r="H6" s="2">
         <v>41744</v>
       </c>
+      <c r="J6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
     </row>
-    <row r="7" spans="6:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F7" s="2" t="s">
+    <row r="7" spans="6:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="5">
+      <c r="G7" s="6"/>
+      <c r="H7" s="3">
         <f>TIME(15,30,20)</f>
         <v>0.64606481481481481</v>
       </c>
+      <c r="J7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
     </row>
-    <row r="8" spans="6:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F8" s="2" t="s">
+    <row r="8" spans="6:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="3" t="s">
+      <c r="G8" s="6"/>
+      <c r="H8" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="J8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="6:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F9" s="2" t="s">
+    <row r="9" spans="6:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="3" t="s">
+      <c r="G9" s="6"/>
+      <c r="H9" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="J9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F10" s="1" t="s">
+    <row r="10" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="F10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="6:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F11" s="2" t="s">
+    <row r="11" spans="6:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="6">
+      <c r="G11" s="6"/>
+      <c r="H11" s="4">
         <v>0.8</v>
       </c>
+      <c r="J11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="6:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F12" s="2" t="s">
+    <row r="12" spans="6:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="6">
+      <c r="G12" s="6"/>
+      <c r="H12" s="4">
         <v>0.3</v>
       </c>
+      <c r="J12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="6:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="6:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F13" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="J13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="24">
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F2:I2"/>
     <mergeCell ref="F10:I10"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="F12:G12"/>
@@ -1449,12 +1627,6 @@
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1793,6 +1965,28 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1052" r:id="rId19" name="Button 28">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!Button28_Click">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>9</xdr:col>
+                    <xdr:colOff>22860</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>22860</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>11</xdr:col>
+                    <xdr:colOff>579120</xdr:colOff>
+                    <xdr:row>14</xdr:row>
+                    <xdr:rowOff>152400</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
   </mc:AlternateContent>

</xml_diff>